<commit_message>
pile and extra hybride
</commit_message>
<xml_diff>
--- a/Checkliste.xlsx
+++ b/Checkliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\OneDrive - Université Laval\Cours\HIV2026\PhotoAlgo\TP2\PhotoAlgo-TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52C0BFD-8A34-4C43-8C54-36494BE036A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C815A2B7-C0BF-497A-929E-571C4ABA2B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85A64DDE-4865-490B-9962-A7310127BEEE}"/>
   </bookViews>
@@ -519,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770E99EC-6A12-45F3-875E-12EC026FB438}">
-  <dimension ref="B1:H28"/>
+  <dimension ref="B1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,17 +535,17 @@
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -559,7 +559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -575,8 +575,11 @@
       <c r="G7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -595,31 +598,37 @@
       <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>14</v>
       </c>
       <c r="E10">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -627,20 +636,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="F15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>21</v>
       </c>
       <c r="F16">
         <v>4</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>